<commit_message>
Cambios masivos en la metodologia
</commit_message>
<xml_diff>
--- a/se/metodología/Libro1.xlsx
+++ b/se/metodología/Libro1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="4965"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="OLE_LINK1" localSheetId="0">Hoja1!$B$3</definedName>
+    <definedName name="OLE_LINK1" localSheetId="0">Hoja1!$C$3</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Disiplinas</t>
   </si>
@@ -46,10 +46,6 @@
   </si>
   <si>
     <t>Modelado del Negocio</t>
-  </si>
-  <si>
-    <t>Modelo de Casos de Uso del Negocio
-Modelo de Objetos del Negicio</t>
   </si>
   <si>
     <t>Vision
@@ -100,19 +96,6 @@
 Estandares de Modelado
 Guia de Estilo para Manuales
 Planilla de Documentos</t>
-  </si>
-  <si>
-    <t>MN-Documento de presentación del cliente (Visión del Cliente).
-MN-Descripción de los Procesos de Negocio.
-MN-Diagrama de Actividades más relevante.
-MN-Diagrama de Casos de Uso del Negocio (solo diagrama)
-MN-Documento de Cruce: Proceso – Actividad – CUN.
-MN-Modelo de dominio.
-MN-Diagrama de contexto.
-MN-Glosario Organizacional.</t>
-  </si>
-  <si>
-    <t>Documento de Especificacion de Requerimientos (De Preliminar a final)</t>
   </si>
   <si>
     <t>AN-Depuración de requerimientos -&gt; Validación 1 a 1
@@ -254,12 +237,168 @@
     <t>• GC-RC: Requerimiento de Cambio
 • GC-RTC: Revisión Técnica Formal del Cambio</t>
   </si>
+  <si>
+    <t>FINAL</t>
+  </si>
+  <si>
+    <t>_x_ Modelo de Casos de Uso del Negocio
+Modelo de Objetos del Negicio</t>
+  </si>
+  <si>
+    <t>_x_ Documento de Especificacion de Requerimientos (De Preliminar a final)</t>
+  </si>
+  <si>
+    <t>_x_ MN-Documento de presentación del cliente (Visión del Cliente).
+_x_ MN-Descripción de los Procesos de Negocio.
+_x_ MN-Diagrama de Actividades más relevante.
+_x_ MN-Diagrama de Casos de Uso del Negocio (solo diagrama)
+MN-Documento de Cruce: Proceso – Actividad – CUN.
+_x_ MN-Modelo de dominio.
+_x_ MN-Diagrama de contexto.
+_x_ MN-Glosario Organizacional.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan de calidad 
+Revisión técnica formal o por pares (RTF) 
+Checklist de verificación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documento de configuración 
+Documento de trazabilidad </t>
+  </si>
+  <si>
+    <t>taringa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Presentación del proyecto 
+o Proceso del Negocio 
+o Documento de Cruce: Proceso-Actividad-CNU 
+o Modelo de dominio de negocio 
+o Glosario Organizacional </t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Documento de relevamiento 
+o Especificación de requerimientos (funcionales, no funcionales) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Casos de uso trazo Grueso 
+o Casos de uso trazo fino 
+o Prototipo de pantalla 
+o Documento de trazabilidad de Proceso-Actividad-CUN 
+o Modelo de análisis (Diagrama de secuencia, Diagrama de Clases) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Modelo de datos (DER) 
+o Modelado de diseño 
+o Definición de Arquitectura </t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Plan de calidad 
+o Revisión técnica formal o por pares (RTF) 
+o Checklist de verificación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Documento de configuración 
+o Documento de trazabilidad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Plan del proyecto 
+o Minutas de reuniones con el cliente 
+o Documento Post-mortem </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento de presentación del Proyecto (Visión).
+Descripción de los Procesos de Negocio.
+Diagrama de Casos de Uso del Negocio (solo diagrama - esboze)
+Diagrama de Actividades más relevante.
+Diagrama de contexto.
+Identificacion de Actores
+Glosario
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Documento de cruce (Proceso – Actividad – CUN)</t>
+    </r>
+  </si>
+  <si>
+    <t>Documento de Relevamiento
+Especificación de Requerimientos
+Especificación Complementaria (No Funcional)</t>
+  </si>
+  <si>
+    <t>Modelo de Datos (DER) – si es necesario –
+Modelo de despliegue
+Modelo de Diseño Diagrama de clases.
+Modelo de Diseño Diagrama de Secuencia.
+Sistemas existentes – Arquitectura existente
+Definición de Arquitectura (General de Software y especifica de componentes)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Diagrama de Casos de Uso (del sistema)
+Documento de Casos de Uso del Sistema – Trazo Grueso
+Documento de Casos de Uso del Sistema – Trazo Fino
+Prototipo de Pantallas
+Diagramas de Secuencia
+Diagrama de Clases
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Depuración de requerimientos -&gt; Validación 1 a 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Documento de trazabilidad (Proceso-Actividad-CUN)</t>
+    </r>
+  </si>
+  <si>
+    <t>Definir metodología
+Documento de Alcance
+Plan del proyecto 
+Minutas de reuniones con el cliente 
+Documento Post-mortem 
+Lista de Riesgos
+Plan de Gestión de Riesgos
+Plan de Iteración</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,8 +421,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +445,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -356,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -367,17 +519,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -679,209 +834,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
+    <col min="2" max="7" width="47.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="120">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="84">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="129.75" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="155.25" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="103.5" customHeight="1">
-      <c r="A2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="3" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="120">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="48">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="78" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="118.5" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="89.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="39" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="78.75" customHeight="1">
-      <c r="A3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="125.25" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="150.75" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="106.5" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="F12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="27" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="51.75" customHeight="1">
-      <c r="A7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="75.75" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="117.75" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="88.5" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="36">
-      <c r="A12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="36">
-      <c r="A13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3" t="s">
-        <v>44</v>
+      <c r="F13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>